<commit_message>
Updated json with build number
</commit_message>
<xml_diff>
--- a/dataFiles/testExcel.xlsx
+++ b/dataFiles/testExcel.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
@@ -446,8 +446,8 @@
     <col width="12.77734375" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
     <col width="11.88671875" bestFit="1" customWidth="1" style="2" min="9" max="10"/>
     <col width="13.88671875" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
-    <col width="8.88671875" customWidth="1" style="2" min="12" max="17"/>
-    <col width="8.88671875" customWidth="1" style="2" min="18" max="16384"/>
+    <col width="8.88671875" customWidth="1" style="2" min="12" max="18"/>
+    <col width="8.88671875" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.6" customFormat="1" customHeight="1" s="1">
@@ -1099,6 +1099,468 @@
         <v>0</v>
       </c>
       <c r="K18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>DAM Smoke Tests UAT</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>01:05:17.790</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>FAILURE</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>72</v>
+      </c>
+      <c r="G19" t="n">
+        <v>71</v>
+      </c>
+      <c r="H19" t="n">
+        <v>6</v>
+      </c>
+      <c r="I19" t="n">
+        <v>65</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>DAM Smoke Tests UAT</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>01:05:17.790</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>FAILURE</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>72</v>
+      </c>
+      <c r="G20" t="n">
+        <v>71</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6</v>
+      </c>
+      <c r="I20" t="n">
+        <v>65</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>DAM Smoke Tests UAT</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>01:05:17.790</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>FAILURE</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>72</v>
+      </c>
+      <c r="G21" t="n">
+        <v>71</v>
+      </c>
+      <c r="H21" t="n">
+        <v>6</v>
+      </c>
+      <c r="I21" t="n">
+        <v>65</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>DAM Smoke Tests UAT</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>01:05:17.790</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>FAILURE</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>72</v>
+      </c>
+      <c r="G22" t="n">
+        <v>71</v>
+      </c>
+      <c r="H22" t="n">
+        <v>6</v>
+      </c>
+      <c r="I22" t="n">
+        <v>65</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>DAM Smoke Tests UAT</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>01:05:17.790</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>FAILURE</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>72</v>
+      </c>
+      <c r="G23" t="n">
+        <v>71</v>
+      </c>
+      <c r="H23" t="n">
+        <v>6</v>
+      </c>
+      <c r="I23" t="n">
+        <v>65</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DAM Smoke Tests UAT</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>01:05:17.790</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>FAILURE</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>72</v>
+      </c>
+      <c r="G24" t="n">
+        <v>71</v>
+      </c>
+      <c r="H24" t="n">
+        <v>6</v>
+      </c>
+      <c r="I24" t="n">
+        <v>65</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>DAM Custom Execution</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>00:01:20.396</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>5</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>5</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>DAM Custom Execution</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2021-03-31</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>00:01:32.984</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" t="n">
+        <v>10</v>
+      </c>
+      <c r="H26" t="n">
+        <v>10</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>DAM Custom Execution</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>82</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2021-03-31</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>00:01:13.715</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>5</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>DAM Smoke Tests UAT</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>13</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2021-02-25</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>01:05:17.790</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>FAILURE</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>72</v>
+      </c>
+      <c r="G28" t="n">
+        <v>71</v>
+      </c>
+      <c r="H28" t="n">
+        <v>6</v>
+      </c>
+      <c r="I28" t="n">
+        <v>65</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>DAM Custom Execution</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>83</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2021-03-31</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>00:01:07.364</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>5</v>
+      </c>
+      <c r="H29" t="n">
+        <v>5</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>DAM Custom Execution</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>84</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2021-03-31</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>00:01:07.256</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>SUCCESS</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>5</v>
+      </c>
+      <c r="G30" t="n">
+        <v>5</v>
+      </c>
+      <c r="H30" t="n">
+        <v>5</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>